<commit_message>
Updated MRR and arranged the testing order in Test Cases for Intermediate Release document.
</commit_message>
<xml_diff>
--- a/Documents/MR Report/MR Report - Project Management App.xlsx
+++ b/Documents/MR Report/MR Report - Project Management App.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -214,9 +214,6 @@
     <t xml:space="preserve">Resolved. </t>
   </si>
   <si>
-    <t xml:space="preserve">Active </t>
-  </si>
-  <si>
     <t xml:space="preserve">The Login button has the wrong text on the button </t>
   </si>
   <si>
@@ -244,9 +241,6 @@
     <t xml:space="preserve">Add a member by clicking their email </t>
   </si>
   <si>
-    <t>Fixed</t>
-  </si>
-  <si>
     <t>ST 10.0</t>
   </si>
   <si>
@@ -278,6 +272,18 @@
   </si>
   <si>
     <t xml:space="preserve">Cant add members </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrong values </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrong values in combo box 3 in create a task </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attempted to retrieve input from user before view is initialized </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start the app </t>
   </si>
 </sst>
 </file>
@@ -382,7 +388,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -436,10 +442,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,7 +994,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>27</v>
@@ -1021,7 +1023,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>18</v>
@@ -1207,7 +1209,7 @@
         <v>63</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1230,13 +1232,13 @@
         <v>61</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>63</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1256,16 +1258,16 @@
         <v>31</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1282,19 +1284,19 @@
         <v>1</v>
       </c>
       <c r="E22" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="G22" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="H22" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H22" s="11" t="s">
-        <v>70</v>
-      </c>
       <c r="I22" s="13" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1314,16 +1316,16 @@
         <v>26</v>
       </c>
       <c r="F23" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="H23" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="I23" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1336,23 +1338,23 @@
       <c r="C24" s="15">
         <v>42430</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="23">
         <v>2</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F24" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="13" t="s">
-        <v>84</v>
-      </c>
       <c r="H24" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1365,23 +1367,23 @@
       <c r="C25" s="15">
         <v>42430</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="23">
         <v>2</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1394,23 +1396,23 @@
       <c r="C26" s="15">
         <v>42430</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="23">
         <v>2</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G26" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="I26" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1423,29 +1425,82 @@
       <c r="C27" s="15">
         <v>42430</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="12">
+        <v>1</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>21</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="15">
+        <v>42431</v>
+      </c>
+      <c r="D28" s="23">
         <v>2</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G27" s="11" t="s">
+      <c r="E28" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <v>22</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="15">
+        <v>42431</v>
+      </c>
+      <c r="D29" s="14">
+        <v>3</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H29" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H27" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="I27" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="26"/>
+      <c r="I29" s="13" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Made minor edits to the Dev Plan and Uploading the new version of the MRR
</commit_message>
<xml_diff>
--- a/Documents/MR Report/MR Report - Project Management App.xlsx
+++ b/Documents/MR Report/MR Report - Project Management App.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="136">
   <si>
     <t>ID</t>
   </si>
@@ -214,6 +214,9 @@
     <t xml:space="preserve">Resolved. </t>
   </si>
   <si>
+    <t xml:space="preserve">Active </t>
+  </si>
+  <si>
     <t xml:space="preserve">The Login button has the wrong text on the button </t>
   </si>
   <si>
@@ -274,16 +277,161 @@
     <t xml:space="preserve">Cant add members </t>
   </si>
   <si>
-    <t xml:space="preserve">Wrong values </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrong values in combo box 3 in create a task </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attempted to retrieve input from user before view is initialized </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start the app </t>
+    <t>Resolved.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input Retrival </t>
+  </si>
+  <si>
+    <t>Attempted to retrieve input from user before view is initialized.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid values </t>
+  </si>
+  <si>
+    <t>Wrong values in a combo box</t>
+  </si>
+  <si>
+    <t>Dr.Tan / Prof. Pham</t>
+  </si>
+  <si>
+    <t>Login to the App</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alert user which screen they are in </t>
+  </si>
+  <si>
+    <t>Everytime a user navagate to screen in the app they should know in which screen they are.</t>
+  </si>
+  <si>
+    <t>Specify to the user that the password should be longer than 4 characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create an account </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create account screen </t>
+  </si>
+  <si>
+    <t>Password Encryption</t>
+  </si>
+  <si>
+    <t>The password should be saved in the database in a encrypted format.</t>
+  </si>
+  <si>
+    <t>Welcome message after logging in</t>
+  </si>
+  <si>
+    <t>There should be some type of welcoming messaged display in the main screen after the user logged in.</t>
+  </si>
+  <si>
+    <t>Merge logging activity and create account activity</t>
+  </si>
+  <si>
+    <t>Create account screen and logging screen should be one screen</t>
+  </si>
+  <si>
+    <t>Load the App</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete unicode character that gets attached to the user data in the database.
+</t>
+  </si>
+  <si>
+    <t>Delete Unicode character</t>
+  </si>
+  <si>
+    <t>Any data that is retrevied from the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viewing of task in the Task List screen </t>
+  </si>
+  <si>
+    <t>Adding of themes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The overall look of the application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When sending an invite to a possible member </t>
+  </si>
+  <si>
+    <t xml:space="preserve">create a task </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the leader is reviewing the task preformed by the member who submited the task </t>
+  </si>
+  <si>
+    <t>Runing the app on devices not specified in the test configuration</t>
+  </si>
+  <si>
+    <t>When leader is viwing the member list of the members in the project</t>
+  </si>
+  <si>
+    <t>Member list activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Besides displaying the members' id, the client requested to have the name of the members as well, displayed. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing app in different devices </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The app must be tested in different devices to make sure that all the views that are part of the app display accordingly. 
+</t>
+  </si>
+  <si>
+    <t>Slider in the task list activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The slider that the leader uses to mark the level of completion of a task, should have the % character besides the number for clarity purposes. 
+</t>
+  </si>
+  <si>
+    <t>Creating a task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The button to submit a task must be disable until the task required fields are filled out completely. 
+</t>
+  </si>
+  <si>
+    <t>Checking email is valid</t>
+  </si>
+  <si>
+    <t>The app must check if the email address given as the user address is valid or active. if it is not active it should be rejected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The app should be able to accommodate user who may have a problem seeing certain colors. the app should offer different theme that provide different color for the app.
+</t>
+  </si>
+  <si>
+    <t>Message in the list task activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There should a message informing the user that there is no task to display if the request to the database provides no task to display. 
+</t>
+  </si>
+  <si>
+    <t>Tutorial screen and main screen</t>
+  </si>
+  <si>
+    <t>User should get from the main screen to the tutorial screen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All </t>
+  </si>
+  <si>
+    <t>ST 1.0 &amp; ST 2.0</t>
+  </si>
+  <si>
+    <t>ST 4.0 &amp; ST 11.0</t>
+  </si>
+  <si>
+    <t>ST.5.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non Functional Requirement </t>
   </si>
 </sst>
 </file>
@@ -388,7 +536,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -441,6 +589,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -752,19 +906,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.85546875" customWidth="1"/>
     <col min="8" max="8" width="19" style="9" bestFit="1" customWidth="1"/>
@@ -994,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>27</v>
@@ -1023,7 +1180,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>18</v>
@@ -1232,7 +1389,7 @@
         <v>61</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>63</v>
@@ -1258,13 +1415,13 @@
         <v>31</v>
       </c>
       <c r="F21" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>70</v>
-      </c>
       <c r="H21" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>64</v>
@@ -1284,19 +1441,19 @@
         <v>1</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1316,16 +1473,16 @@
         <v>26</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1342,16 +1499,16 @@
         <v>2</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G24" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="I24" s="13" t="s">
         <v>64</v>
@@ -1371,19 +1528,19 @@
         <v>2</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1400,19 +1557,19 @@
         <v>2</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1429,19 +1586,19 @@
         <v>1</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1461,16 +1618,16 @@
         <v>24</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -1487,27 +1644,437 @@
         <v>3</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G29" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I29" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H29" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>64</v>
-      </c>
+    </row>
+    <row r="30" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <v>23</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D30" s="19">
+        <v>4</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I30" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <v>24</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D31" s="19">
+        <v>4</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="I31" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
+        <v>25</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D32" s="19">
+        <v>4</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
+        <v>26</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D33" s="19">
+        <v>4</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I33" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <v>27</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D34" s="19">
+        <v>4</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="I34" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
+        <v>28</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D35" s="19">
+        <v>4</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H35" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="I35" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
+        <v>29</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D36" s="19">
+        <v>4</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I36" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>30</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D37" s="19">
+        <v>4</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="I37" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="13">
+        <v>31</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D38" s="19">
+        <v>4</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="I38" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
+        <v>32</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D39" s="19">
+        <v>4</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="I39" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
+        <v>33</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D40" s="19">
+        <v>4</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="I40" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <v>34</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D41" s="19">
+        <v>4</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="G41" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="H41" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="13">
+        <v>35</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D42" s="23">
+        <v>2</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="H42" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="I42" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="13">
+        <v>36</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="15">
+        <v>42434</v>
+      </c>
+      <c r="D43" s="19">
+        <v>4</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="G43" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="I43" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F44" s="9"/>
+      <c r="I44" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup scale="59" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated version of MRR and Test Plan
</commit_message>
<xml_diff>
--- a/Documents/MR Report/MR Report - Project Management App.xlsx
+++ b/Documents/MR Report/MR Report - Project Management App.xlsx
@@ -1063,8 +1063,8 @@
   </sheetPr>
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,7 +2011,7 @@
         <v>91</v>
       </c>
       <c r="I36" s="25" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2475,7 +2475,7 @@
         <v>155</v>
       </c>
       <c r="I52" s="24" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated MRR and Made some minor edits to Database Design Doc
</commit_message>
<xml_diff>
--- a/Documents/MR Report/MR Report - Project Management App.xlsx
+++ b/Documents/MR Report/MR Report - Project Management App.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="188">
   <si>
     <t>ID</t>
   </si>
@@ -574,6 +574,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Create task and Remove members</t>
+  </si>
+  <si>
+    <t>Main Menu button now takes user to Theme</t>
+  </si>
+  <si>
+    <t>Click the main menu button</t>
+  </si>
+  <si>
+    <t>Main Menu Button</t>
   </si>
 </sst>
 </file>
@@ -1061,10 +1070,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2679,6 +2688,35 @@
       </c>
       <c r="I59" s="24" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="11">
+        <v>53</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="15">
+        <v>42463</v>
+      </c>
+      <c r="D60" s="28">
+        <v>4</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="F60" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="G60" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="I60" s="24" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated MRR and Draft of User Manual
</commit_message>
<xml_diff>
--- a/Documents/MR Report/MR Report - Project Management App.xlsx
+++ b/Documents/MR Report/MR Report - Project Management App.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="192">
   <si>
     <t>ID</t>
   </si>
@@ -583,6 +583,18 @@
   </si>
   <si>
     <t>Main Menu Button</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a task with two or more words </t>
+  </si>
+  <si>
+    <t>When a task is created with more than two words, the action of submitting a task will not update</t>
+  </si>
+  <si>
+    <t>ST 5.0, ST. 7.0 &amp; ST. 8.0</t>
   </si>
 </sst>
 </file>
@@ -688,7 +700,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -756,6 +768,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1070,10 +1088,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2352,8 +2370,8 @@
       <c r="C48" s="15">
         <v>42451</v>
       </c>
-      <c r="D48" s="19">
-        <v>4</v>
+      <c r="D48" s="14">
+        <v>3</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>148</v>
@@ -2439,8 +2457,8 @@
       <c r="C51" s="16">
         <v>42423</v>
       </c>
-      <c r="D51" s="26">
-        <v>4</v>
+      <c r="D51" s="31">
+        <v>3</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>181</v>
@@ -2629,7 +2647,7 @@
         <v>166</v>
       </c>
       <c r="I57" s="24" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2671,8 +2689,8 @@
       <c r="C59" s="27">
         <v>42425</v>
       </c>
-      <c r="D59" s="28">
-        <v>4</v>
+      <c r="D59" s="30">
+        <v>3</v>
       </c>
       <c r="E59" s="24" t="s">
         <v>177</v>
@@ -2716,7 +2734,36 @@
         <v>186</v>
       </c>
       <c r="I60" s="24" t="s">
-        <v>129</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A61" s="11">
+        <v>54</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="15">
+        <v>42104</v>
+      </c>
+      <c r="D61" s="28">
+        <v>2</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="G61" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="I61" s="24" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates in the MRR and SRS
</commit_message>
<xml_diff>
--- a/Documents/MR Report/MR Report - Project Management App.xlsx
+++ b/Documents/MR Report/MR Report - Project Management App.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="193">
   <si>
     <t>ID</t>
   </si>
@@ -595,6 +595,9 @@
   </si>
   <si>
     <t>ST 5.0, ST. 7.0 &amp; ST. 8.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed. </t>
   </si>
 </sst>
 </file>
@@ -766,14 +769,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1090,8 +1093,8 @@
   </sheetPr>
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,10 +1111,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="20" t="s">
         <v>40</v>
       </c>
@@ -1864,7 +1867,7 @@
         <v>91</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -2457,7 +2460,7 @@
       <c r="C51" s="16">
         <v>42423</v>
       </c>
-      <c r="D51" s="31">
+      <c r="D51" s="30">
         <v>3</v>
       </c>
       <c r="E51" s="11" t="s">
@@ -2589,7 +2592,7 @@
         <v>155</v>
       </c>
       <c r="I55" s="24" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -2689,7 +2692,7 @@
       <c r="C59" s="27">
         <v>42425</v>
       </c>
-      <c r="D59" s="30">
+      <c r="D59" s="29">
         <v>3</v>
       </c>
       <c r="E59" s="24" t="s">
@@ -2747,8 +2750,8 @@
       <c r="C61" s="15">
         <v>42104</v>
       </c>
-      <c r="D61" s="28">
-        <v>2</v>
+      <c r="D61" s="29">
+        <v>3</v>
       </c>
       <c r="E61" s="24" t="s">
         <v>191</v>
@@ -2763,7 +2766,7 @@
         <v>189</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>64</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MRR edits and Test Doc edits
</commit_message>
<xml_diff>
--- a/Documents/MR Report/MR Report - Project Management App.xlsx
+++ b/Documents/MR Report/MR Report - Project Management App.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="204">
   <si>
     <t>ID</t>
   </si>
@@ -407,9 +407,6 @@
     <t xml:space="preserve">Non Functional Requirement </t>
   </si>
   <si>
-    <t>Fixed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fixed </t>
   </si>
   <si>
@@ -598,13 +595,49 @@
   </si>
   <si>
     <t xml:space="preserve">Resolved </t>
+  </si>
+  <si>
+    <t>Professor Pham</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Version Number</t>
+  </si>
+  <si>
+    <t>Add the version number to the app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website message </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add a happy message when member accepts invatations </t>
+  </si>
+  <si>
+    <t>Invite a member</t>
+  </si>
+  <si>
+    <t>Leader remove a member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the user is a leader remove a member should work </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A and Android Design </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolved by the use of error handeling  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A, if user use an invalid email user wont be able to accept emails </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,6 +683,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -703,7 +742,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -773,6 +812,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1091,10 +1133,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,10 +1153,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="20" t="s">
         <v>40</v>
       </c>
@@ -1310,7 +1352,7 @@
         <v>15</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>16</v>
@@ -1867,7 +1909,7 @@
         <v>91</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -1896,7 +1938,7 @@
         <v>95</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>64</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1925,7 +1967,7 @@
         <v>95</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1954,7 +1996,7 @@
         <v>91</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2006,7 +2048,7 @@
         <v>104</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H35" s="24" t="s">
         <v>105</v>
@@ -2041,7 +2083,7 @@
         <v>91</v>
       </c>
       <c r="I36" s="25" t="s">
-        <v>130</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2064,13 +2106,13 @@
         <v>121</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H37" s="24" t="s">
         <v>106</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2093,16 +2135,16 @@
         <v>107</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H38" s="24" t="s">
         <v>108</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="126" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>32</v>
       </c>
@@ -2127,11 +2169,11 @@
       <c r="H39" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="I39" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>33</v>
       </c>
@@ -2151,13 +2193,13 @@
         <v>118</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H40" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="I40" s="25" t="s">
-        <v>64</v>
+      <c r="I40" s="24" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
@@ -2186,7 +2228,7 @@
         <v>111</v>
       </c>
       <c r="I41" s="25" t="s">
-        <v>64</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
@@ -2215,7 +2257,7 @@
         <v>112</v>
       </c>
       <c r="I42" s="25" t="s">
-        <v>64</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2238,10 +2280,10 @@
         <v>113</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I43" s="25" t="s">
         <v>85</v>
@@ -2267,10 +2309,10 @@
         <v>118</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I44" s="13" t="s">
         <v>85</v>
@@ -2290,16 +2332,16 @@
         <v>4</v>
       </c>
       <c r="E45" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F45" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="F45" s="24" t="s">
+      <c r="G45" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H45" s="11" t="s">
         <v>137</v>
-      </c>
-      <c r="G45" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>138</v>
       </c>
       <c r="I45" s="25" t="s">
         <v>85</v>
@@ -2319,19 +2361,19 @@
         <v>4</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I46" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2351,13 +2393,13 @@
         <v>127</v>
       </c>
       <c r="F47" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G47" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="G47" s="24" t="s">
-        <v>135</v>
-      </c>
       <c r="H47" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I47" s="25" t="s">
         <v>85</v>
@@ -2377,19 +2419,19 @@
         <v>3</v>
       </c>
       <c r="E48" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="F48" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="F48" s="24" t="s">
+      <c r="G48" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="G48" s="11" t="s">
+      <c r="H48" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="H48" s="11" t="s">
-        <v>151</v>
-      </c>
       <c r="I48" s="25" t="s">
-        <v>130</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2406,19 +2448,19 @@
         <v>4</v>
       </c>
       <c r="E49" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F49" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="H49" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="F49" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="G49" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>154</v>
-      </c>
       <c r="I49" s="24" t="s">
-        <v>64</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2435,19 +2477,19 @@
         <v>4</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>64</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2464,19 +2506,19 @@
         <v>3</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2484,7 +2526,7 @@
         <v>45</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C52" s="27">
         <v>42424</v>
@@ -2493,19 +2535,19 @@
         <v>4</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H52" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I52" s="24" t="s">
-        <v>129</v>
+        <v>187</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2522,19 +2564,19 @@
         <v>4</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F53" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="G53" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="G53" s="24" t="s">
-        <v>160</v>
-      </c>
       <c r="H53" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I53" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2557,13 +2599,13 @@
         <v>118</v>
       </c>
       <c r="G54" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="H54" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="H54" s="24" t="s">
-        <v>166</v>
-      </c>
       <c r="I54" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -2580,19 +2622,19 @@
         <v>4</v>
       </c>
       <c r="E55" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F55" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="G55" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="G55" s="24" t="s">
-        <v>168</v>
-      </c>
       <c r="H55" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I55" s="24" t="s">
-        <v>130</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -2609,19 +2651,19 @@
         <v>4</v>
       </c>
       <c r="E56" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F56" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G56" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="G56" s="24" t="s">
+      <c r="H56" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="H56" s="24" t="s">
-        <v>171</v>
-      </c>
       <c r="I56" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
@@ -2644,13 +2686,13 @@
         <v>118</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H57" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I57" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2667,19 +2709,19 @@
         <v>4</v>
       </c>
       <c r="E58" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="F58" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F58" s="24" t="s">
+      <c r="G58" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="G58" s="24" t="s">
+      <c r="H58" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="H58" s="24" t="s">
-        <v>176</v>
-      </c>
       <c r="I58" s="24" t="s">
-        <v>64</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2696,19 +2738,19 @@
         <v>3</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G59" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="H59" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="H59" s="24" t="s">
-        <v>183</v>
-      </c>
       <c r="I59" s="24" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -2725,19 +2767,19 @@
         <v>4</v>
       </c>
       <c r="E60" s="24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F60" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="G60" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I60" s="24" t="s">
         <v>187</v>
-      </c>
-      <c r="G60" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="I60" s="24" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="63" x14ac:dyDescent="0.25">
@@ -2754,20 +2796,122 @@
         <v>3</v>
       </c>
       <c r="E61" s="24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F61" s="24" t="s">
         <v>118</v>
       </c>
       <c r="G61" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I61" s="24" t="s">
         <v>63</v>
       </c>
+    </row>
+    <row r="62" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="11">
+        <v>55</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="C62" s="15">
+        <v>42485</v>
+      </c>
+      <c r="D62" s="28">
+        <v>4</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="G62" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="H62" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="I62" s="24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="11">
+        <v>56</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" s="15">
+        <v>42485</v>
+      </c>
+      <c r="D63" s="29">
+        <v>3</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="G63" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="I63" s="24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="11">
+        <v>57</v>
+      </c>
+      <c r="B64" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" s="15">
+        <v>42485</v>
+      </c>
+      <c r="D64" s="28">
+        <v>4</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="G64" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="H64" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="I64" s="24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="15"/>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="11"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="15"/>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="11"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>